<commit_message>
page model correction ratio
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>model type</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>first_try</t>
+  </si>
+  <si>
+    <t>page/record</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>record</t>
   </si>
 </sst>
 </file>
@@ -407,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,18 +427,19 @@
     <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -440,37 +450,40 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,98 +493,133 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.05</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>6</v>
-      </c>
-      <c r="G2">
-        <v>16</v>
       </c>
       <c r="H2">
         <v>16</v>
       </c>
       <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
         <v>3.1314782798290197E-2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>4.9022734165191598E-3</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.96219600000000005</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.95932899999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0.05</v>
       </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>7.9865917559999999E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.89944000000000002</v>
+      </c>
+      <c r="M3">
+        <v>0.89479797271749995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="b">
+      <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.05</v>
       </c>
-      <c r="F4">
+      <c r="G4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="b">
+      <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="b">
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix entity correct ratio
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>model type</t>
   </si>
@@ -26,18 +26,9 @@
     <t>id</t>
   </si>
   <si>
-    <t>LSTM</t>
-  </si>
-  <si>
     <t>bidirectional</t>
   </si>
   <si>
-    <t>LSTM-2layer</t>
-  </si>
-  <si>
-    <t>LSTM CRF</t>
-  </si>
-  <si>
     <t>Best epoch</t>
   </si>
   <si>
@@ -65,16 +56,61 @@
     <t>alias</t>
   </si>
   <si>
-    <t>first_try</t>
-  </si>
-  <si>
     <t>page/record</t>
   </si>
   <si>
-    <t>page</t>
-  </si>
-  <si>
     <t>record</t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>encoder</t>
+  </si>
+  <si>
+    <t>bert</t>
+  </si>
+  <si>
+    <t>lstm</t>
+  </si>
+  <si>
+    <t>batch_test</t>
+  </si>
+  <si>
+    <t>correct ratio train</t>
+  </si>
+  <si>
+    <t>correct ratio cv</t>
+  </si>
+  <si>
+    <t>entity correct ratio train</t>
+  </si>
+  <si>
+    <t>entity correct ratio cv</t>
+  </si>
+  <si>
+    <t>data size</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>polyglot MCP</t>
+  </si>
+  <si>
+    <t>lstmcrf</t>
+  </si>
+  <si>
+    <t>train loss</t>
+  </si>
+  <si>
+    <t>cv loss</t>
+  </si>
+  <si>
+    <t>0.284485177(bug fixed)</t>
   </si>
 </sst>
 </file>
@@ -416,215 +452,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.1796875" customWidth="1"/>
+    <col min="14" max="14" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.453125" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" customWidth="1"/>
+    <col min="17" max="17" width="26.36328125" customWidth="1"/>
+    <col min="18" max="18" width="19.81640625" customWidth="1"/>
+    <col min="19" max="19" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="U1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.05</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
       </c>
       <c r="I2">
         <v>16</v>
       </c>
       <c r="J2">
-        <v>3.1314782798290197E-2</v>
+        <v>8</v>
       </c>
       <c r="K2">
-        <v>4.9022734165191598E-3</v>
-      </c>
-      <c r="L2">
-        <v>0.96219600000000005</v>
-      </c>
-      <c r="M2">
-        <v>0.95932899999999999</v>
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <v>0.12224528699999999</v>
+      </c>
+      <c r="P2">
+        <v>0.12159761018</v>
+      </c>
+      <c r="Q2">
+        <v>5.1228999999999997E-2</v>
+      </c>
+      <c r="R2">
+        <v>5.1679857000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="b">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0.05</v>
-      </c>
       <c r="H3">
-        <v>20</v>
+        <v>2E-3</v>
       </c>
       <c r="I3">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>7.9865917559999999E-2</v>
-      </c>
-      <c r="L3">
-        <v>0.89944000000000002</v>
-      </c>
-      <c r="M3">
-        <v>0.89479797271749995</v>
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>0.2820066</v>
+      </c>
+      <c r="P3">
+        <v>0.28327128896999998</v>
+      </c>
+      <c r="Q3">
+        <v>9.1211799999999996E-2</v>
+      </c>
+      <c r="R3">
+        <v>9.0816999999999995E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="b">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2E-3</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>0.27743916400000002</v>
+      </c>
+      <c r="P4">
+        <v>0.27400341239999998</v>
+      </c>
+      <c r="Q4">
+        <v>8.7652567000000001E-2</v>
+      </c>
+      <c r="R4">
+        <v>8.7831548999999995E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0.05</v>
-      </c>
-      <c r="G4">
+      <c r="H5">
+        <v>2E-3</v>
+      </c>
+      <c r="I5">
         <v>6</v>
       </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>0.27927225999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.27846284999999998</v>
+      </c>
+      <c r="Q5">
+        <v>9.2632479000000004E-2</v>
+      </c>
+      <c r="R5">
+        <v>9.2950199999999997E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="b">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="b">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0.05</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="H6">
+        <v>2E-3</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="O6">
+        <v>0.27882899999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.27958739999999999</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6">
+        <v>0.28159775096599998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
save model and continue to train
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>model type</t>
   </si>
@@ -120,13 +120,25 @@
   </si>
   <si>
     <t>lstm-crf</t>
+  </si>
+  <si>
+    <t>0.7695（非cvloss最低）</t>
+  </si>
+  <si>
+    <t>Page Model adjustment</t>
+  </si>
+  <si>
+    <t>0.834（最后一轮）</t>
+  </si>
+  <si>
+    <t>没算出来</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +159,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +177,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,11 +199,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -483,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,7 +532,7 @@
     <col min="13" max="13" width="18.453125" customWidth="1"/>
     <col min="14" max="14" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.453125" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" customWidth="1"/>
+    <col min="16" max="16" width="25.26953125" customWidth="1"/>
     <col min="17" max="17" width="26.36328125" customWidth="1"/>
     <col min="18" max="18" width="19.81640625" customWidth="1"/>
     <col min="19" max="19" width="22.26953125" bestFit="1" customWidth="1"/>
@@ -858,6 +885,21 @@
       <c r="K9">
         <v>50</v>
       </c>
+      <c r="L9">
+        <v>4.2110000000000002E-2</v>
+      </c>
+      <c r="M9">
+        <v>6.3149738999999996E-2</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>0.79850923419999997</v>
+      </c>
+      <c r="P9">
+        <v>0.78533897470000003</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -887,6 +929,21 @@
       <c r="K10">
         <v>50</v>
       </c>
+      <c r="L10">
+        <v>28.7268574</v>
+      </c>
+      <c r="M10">
+        <v>10.298999999999999</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <v>0.80765600000000004</v>
+      </c>
+      <c r="P10">
+        <v>0.79395800000000005</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
@@ -914,7 +971,28 @@
         <v>4</v>
       </c>
       <c r="K11">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>0.29234789999999999</v>
+      </c>
+      <c r="M11">
+        <v>0.57277294999999995</v>
+      </c>
+      <c r="N11">
+        <v>24</v>
+      </c>
+      <c r="O11">
+        <v>0.77044400000000002</v>
+      </c>
+      <c r="P11">
+        <v>0.76546593730000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.71631615999999998</v>
+      </c>
+      <c r="R11">
+        <v>0.71554799999999996</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
@@ -944,6 +1022,228 @@
       </c>
       <c r="K12">
         <v>50</v>
+      </c>
+      <c r="L12">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="M12">
+        <v>5.85976E-2</v>
+      </c>
+      <c r="N12">
+        <v>29</v>
+      </c>
+      <c r="O12">
+        <v>0.80510000000000004</v>
+      </c>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2E-3</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>50</v>
+      </c>
+      <c r="L14">
+        <v>28.7268574</v>
+      </c>
+      <c r="M14">
+        <v>10.298999999999999</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14">
+        <v>0.80765600000000004</v>
+      </c>
+      <c r="P14">
+        <v>0.79395800000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="I15">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>50</v>
+      </c>
+      <c r="L15">
+        <v>13.889988000000001</v>
+      </c>
+      <c r="M15">
+        <v>13.306174</v>
+      </c>
+      <c r="O15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="I16">
+        <v>16</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>66</v>
+      </c>
+      <c r="O16">
+        <v>0.85229999999999995</v>
+      </c>
+      <c r="P16">
+        <v>0.784335334</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>2E-3</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+      <c r="L19">
+        <v>0.29234789999999999</v>
+      </c>
+      <c r="M19">
+        <v>0.57277294999999995</v>
+      </c>
+      <c r="N19">
+        <v>24</v>
+      </c>
+      <c r="O19">
+        <v>0.77044400000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.76546593730000001</v>
+      </c>
+      <c r="Q19">
+        <v>0.71631615999999998</v>
+      </c>
+      <c r="R19">
+        <v>0.71554799999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2E-3</v>
+      </c>
+      <c r="I20">
+        <v>16</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="R20">
+        <v>0.71554799999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backup before encoder supporting device
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="43">
   <si>
     <t>model type</t>
   </si>
@@ -141,13 +141,16 @@
   </si>
   <si>
     <t>Record Model</t>
+  </si>
+  <si>
+    <t>polyglot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +185,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -221,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -230,6 +253,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -534,10 +559,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,7 +572,7 @@
     <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.54296875" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
@@ -1153,6 +1180,21 @@
       <c r="L15">
         <v>50</v>
       </c>
+      <c r="M15">
+        <v>18.235810000000001</v>
+      </c>
+      <c r="N15">
+        <v>8.7282989999999998</v>
+      </c>
+      <c r="O15">
+        <v>49</v>
+      </c>
+      <c r="P15">
+        <v>0.87408399999999997</v>
+      </c>
+      <c r="Q15">
+        <v>0.82613400000000003</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
@@ -1385,6 +1427,227 @@
       </c>
       <c r="R22">
         <v>0.89031136</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>20200301</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>2E-3</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>32</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>82</v>
+      </c>
+      <c r="O23">
+        <v>74</v>
+      </c>
+      <c r="P23">
+        <v>0.79552330000000004</v>
+      </c>
+      <c r="Q23">
+        <v>0.78578700000000001</v>
+      </c>
+      <c r="R23">
+        <v>0.89349478999999998</v>
+      </c>
+      <c r="S23">
+        <v>0.88479154900000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>20200305</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2E-3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>64</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>141</v>
+      </c>
+      <c r="M24">
+        <v>7.5662240000000001</v>
+      </c>
+      <c r="N24">
+        <v>3.190741</v>
+      </c>
+      <c r="O24">
+        <v>115</v>
+      </c>
+      <c r="P24">
+        <v>0.79114865999999995</v>
+      </c>
+      <c r="Q24">
+        <v>0.77766900000000005</v>
+      </c>
+      <c r="R24">
+        <v>0.88866647889999995</v>
+      </c>
+      <c r="S24">
+        <v>0.87588900000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>202003012</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>2E-3</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>64</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>60</v>
+      </c>
+      <c r="M26">
+        <v>8.1295697899999997</v>
+      </c>
+      <c r="N26">
+        <v>4.5420870000000004</v>
+      </c>
+      <c r="O26">
+        <v>60</v>
+      </c>
+      <c r="P26">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="Q26">
+        <v>0.65255275999999995</v>
+      </c>
+      <c r="R26">
+        <v>0.81064076799999996</v>
+      </c>
+      <c r="S26">
+        <v>0.80737700000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>202003014</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2</v>
+      </c>
+      <c r="J27" s="3">
+        <v>64</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>50</v>
+      </c>
+      <c r="M27">
+        <v>0.57762796954999995</v>
+      </c>
+      <c r="N27">
+        <v>0.57193222376999997</v>
+      </c>
+      <c r="O27">
+        <v>50</v>
+      </c>
+      <c r="P27">
+        <v>0.57762796954999995</v>
+      </c>
+      <c r="Q27">
+        <v>0.57193222376999997</v>
+      </c>
+      <c r="R27">
+        <v>0.73700476999999998</v>
+      </c>
+      <c r="S27">
+        <v>0.7361482855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>